<commit_message>
feat: improve excel read/write support for datasets with MultiIndex columns
</commit_message>
<xml_diff>
--- a/tests/cli/macpie/merge/small_expected_results.xlsx
+++ b/tests/cli/macpie/merge/small_expected_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alee7/ucsf/git/macpie/tests/cli/merge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alee7/ucsf/git/macpie/tests/cli/macpie/merge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C36A689-BB1E-9447-9893-4BBC019E3173}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08387287-6617-9C4E-B400-4FBDB65D4065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16540" yWindow="5180" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="1060" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MERGED_RESULTS" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
     <sheet name="_sheets" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MERGED_RESULTS!$B$2:$S$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MERGED_RESULTS!$A$2:$R$27</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="77">
   <si>
     <t>small</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>instr3_all</t>
-  </si>
-  <si>
-    <t>Original_Order</t>
   </si>
   <si>
     <t>PIDN</t>
@@ -656,55 +653,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="L1" s="5"/>
+      <c r="M1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="5"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -724,7 +721,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -742,7 +739,7 @@
         <v>8</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>4</v>
@@ -759,45 +756,39 @@
       <c r="R2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>83506</v>
       </c>
-      <c r="C3" s="2">
+      <c r="B3" s="2">
         <v>36452</v>
       </c>
+      <c r="C3">
+        <v>178771</v>
+      </c>
       <c r="D3">
-        <v>178771</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>212592</v>
       </c>
-      <c r="C4" s="2">
+      <c r="B4" s="2">
         <v>35912</v>
       </c>
+      <c r="C4">
+        <v>877207</v>
+      </c>
       <c r="D4">
-        <v>877207</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -806,34 +797,34 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
         <v>212592</v>
       </c>
-      <c r="I4" s="2">
+      <c r="H4" s="2">
         <v>35912</v>
       </c>
+      <c r="I4">
+        <v>500861</v>
+      </c>
       <c r="J4">
-        <v>500861</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4">
         <v>212592</v>
       </c>
-      <c r="O4" s="2">
+      <c r="N4" s="2">
         <v>35912</v>
       </c>
+      <c r="O4">
+        <v>603240</v>
+      </c>
       <c r="P4">
-        <v>603240</v>
+        <v>1</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -841,22 +832,19 @@
       <c r="R4">
         <v>1</v>
       </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>225430</v>
       </c>
-      <c r="C5" s="2">
+      <c r="B5" s="2">
         <v>35547</v>
       </c>
+      <c r="C5">
+        <v>925508</v>
+      </c>
       <c r="D5">
-        <v>925508</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -865,149 +853,134 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
         <v>225430</v>
       </c>
-      <c r="I5" s="2">
+      <c r="H5" s="2">
         <v>35547</v>
       </c>
+      <c r="I5">
+        <v>888874</v>
+      </c>
       <c r="J5">
-        <v>888874</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
         <v>225430</v>
       </c>
-      <c r="O5" s="2">
+      <c r="N5" s="2">
         <v>35547</v>
       </c>
+      <c r="O5">
+        <v>341269</v>
+      </c>
       <c r="P5">
-        <v>341269</v>
+        <v>2</v>
       </c>
       <c r="Q5">
-        <v>2</v>
+        <v>-6</v>
       </c>
       <c r="R5">
         <v>-6</v>
       </c>
-      <c r="S5">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>250494</v>
       </c>
-      <c r="C6" s="2">
+      <c r="B6" s="2">
         <v>35614</v>
       </c>
+      <c r="C6">
+        <v>499743</v>
+      </c>
       <c r="D6">
-        <v>499743</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>0.5</v>
       </c>
-      <c r="F6">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>291649</v>
+      </c>
+      <c r="B7" s="2">
+        <v>35900</v>
+      </c>
+      <c r="C7">
+        <v>779189</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>298326</v>
+      </c>
+      <c r="B8" s="2">
+        <v>35679</v>
+      </c>
+      <c r="C8">
+        <v>137398</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>304442</v>
+      </c>
+      <c r="B9" s="2">
+        <v>35666</v>
+      </c>
+      <c r="C9">
+        <v>515744</v>
+      </c>
+      <c r="D9">
         <v>0</v>
       </c>
-      <c r="G6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>291649</v>
-      </c>
-      <c r="C7" s="2">
-        <v>35900</v>
-      </c>
-      <c r="D7">
-        <v>779189</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>298326</v>
-      </c>
-      <c r="C8" s="2">
-        <v>35679</v>
-      </c>
-      <c r="D8">
-        <v>137398</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>304442</v>
-      </c>
-      <c r="C9" s="2">
-        <v>35666</v>
-      </c>
-      <c r="D9">
-        <v>515744</v>
-      </c>
       <c r="E9">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="F9">
         <v>-9</v>
       </c>
-      <c r="G9">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>328347</v>
       </c>
-      <c r="C10" s="2">
+      <c r="B10" s="2">
         <v>39230</v>
       </c>
+      <c r="C10">
+        <v>187481</v>
+      </c>
       <c r="D10">
-        <v>187481</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1015,45 +988,39 @@
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>402824</v>
+      </c>
+      <c r="B11" s="2">
+        <v>35593</v>
+      </c>
+      <c r="C11">
+        <v>250964</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>402824</v>
-      </c>
-      <c r="C11" s="2">
-        <v>35593</v>
-      </c>
-      <c r="D11">
-        <v>250964</v>
-      </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.5</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>476359</v>
+      </c>
+      <c r="B12" s="2">
+        <v>35982</v>
+      </c>
+      <c r="C12">
+        <v>185271</v>
+      </c>
+      <c r="D12">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>476359</v>
-      </c>
-      <c r="C12" s="2">
-        <v>35982</v>
-      </c>
-      <c r="D12">
-        <v>185271</v>
       </c>
       <c r="E12">
         <v>0.5</v>
@@ -1061,223 +1028,202 @@
       <c r="F12">
         <v>0.5</v>
       </c>
-      <c r="G12">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>492020</v>
+      </c>
+      <c r="B13" s="2">
+        <v>35617</v>
+      </c>
+      <c r="C13">
+        <v>785354</v>
+      </c>
+      <c r="D13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>492020</v>
-      </c>
-      <c r="C13" s="2">
-        <v>35617</v>
-      </c>
-      <c r="D13">
-        <v>785354</v>
-      </c>
       <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>525567</v>
+      </c>
+      <c r="B14" s="2">
+        <v>36410</v>
+      </c>
+      <c r="C14">
+        <v>104467</v>
+      </c>
+      <c r="D14">
         <v>0.5</v>
       </c>
-      <c r="F13">
+      <c r="E14">
         <v>0</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14">
+      <c r="F14">
+        <v>0.5</v>
+      </c>
+      <c r="G14">
         <v>525567</v>
       </c>
-      <c r="C14" s="2">
+      <c r="H14" s="2">
         <v>36410</v>
       </c>
-      <c r="D14">
-        <v>104467</v>
-      </c>
-      <c r="E14">
+      <c r="I14">
+        <v>671290</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>531077</v>
+      </c>
+      <c r="B15" s="2">
+        <v>35708</v>
+      </c>
+      <c r="C15">
+        <v>819165</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>551893</v>
+      </c>
+      <c r="B16" s="2">
+        <v>36069</v>
+      </c>
+      <c r="C16">
+        <v>617550</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>584891</v>
+      </c>
+      <c r="B17" s="2">
+        <v>37230</v>
+      </c>
+      <c r="C17">
+        <v>488606</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
         <v>0.5</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0.5</v>
-      </c>
-      <c r="H14">
-        <v>525567</v>
-      </c>
-      <c r="I14" s="2">
-        <v>36410</v>
-      </c>
-      <c r="J14">
-        <v>671290</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>531077</v>
-      </c>
-      <c r="C15" s="2">
-        <v>35708</v>
-      </c>
-      <c r="D15">
-        <v>819165</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>551893</v>
-      </c>
-      <c r="C16" s="2">
-        <v>36069</v>
-      </c>
-      <c r="D16">
-        <v>617550</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
         <v>584891</v>
       </c>
-      <c r="C17" s="2">
+      <c r="H17" s="2">
         <v>37230</v>
       </c>
-      <c r="D17">
-        <v>488606</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0.5</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>584891</v>
-      </c>
-      <c r="I17" s="2">
-        <v>37230</v>
+      <c r="I17">
+        <v>190736</v>
       </c>
       <c r="J17">
-        <v>190736</v>
+        <v>3</v>
       </c>
       <c r="K17">
         <v>3</v>
       </c>
       <c r="L17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
         <v>584891</v>
       </c>
-      <c r="O17" s="2">
+      <c r="N17" s="2">
         <v>37230</v>
       </c>
+      <c r="O17">
+        <v>994547</v>
+      </c>
       <c r="P17">
-        <v>994547</v>
+        <v>2</v>
       </c>
       <c r="Q17">
-        <v>2</v>
+        <v>-6</v>
       </c>
       <c r="R17">
         <v>-6</v>
       </c>
-      <c r="S17">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>645686</v>
       </c>
-      <c r="C18" s="2">
+      <c r="B18" s="2">
         <v>37435</v>
       </c>
-      <c r="D18">
+      <c r="C18">
         <v>613114</v>
       </c>
-      <c r="H18">
+      <c r="G18">
         <v>645686</v>
       </c>
-      <c r="I18" s="2">
+      <c r="H18" s="2">
         <v>37435</v>
       </c>
-      <c r="J18">
+      <c r="I18">
         <v>877446</v>
       </c>
-      <c r="N18">
+      <c r="M18">
         <v>645686</v>
       </c>
-      <c r="O18" s="2">
+      <c r="N18" s="2">
         <v>37435</v>
       </c>
-      <c r="P18">
+      <c r="O18">
         <v>768903</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>650255</v>
       </c>
-      <c r="C19" s="2">
+      <c r="B19" s="2">
         <v>35680</v>
       </c>
+      <c r="C19">
+        <v>207261</v>
+      </c>
       <c r="D19">
-        <v>207261</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -1285,68 +1231,59 @@
       <c r="F19">
         <v>2</v>
       </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>657201</v>
       </c>
-      <c r="C20" s="2">
+      <c r="B20" s="2">
         <v>35837</v>
       </c>
+      <c r="C20">
+        <v>715059</v>
+      </c>
       <c r="D20">
-        <v>715059</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="F20">
         <v>-9</v>
       </c>
-      <c r="G20">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>674946</v>
       </c>
-      <c r="C21" s="2">
+      <c r="B21" s="2">
         <v>35431</v>
       </c>
+      <c r="C21">
+        <v>534853</v>
+      </c>
       <c r="D21">
-        <v>534853</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22">
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>690264</v>
       </c>
-      <c r="C22" s="2">
+      <c r="B22" s="2">
         <v>35990</v>
       </c>
+      <c r="C22">
+        <v>497023</v>
+      </c>
       <c r="D22">
-        <v>497023</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1354,45 +1291,39 @@
       <c r="F22">
         <v>2</v>
       </c>
-      <c r="G22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23">
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>855273</v>
       </c>
-      <c r="C23" s="2">
+      <c r="B23" s="2">
         <v>35607</v>
       </c>
+      <c r="C23">
+        <v>744447</v>
+      </c>
       <c r="D23">
-        <v>744447</v>
+        <v>0.5</v>
       </c>
       <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <v>0.5</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24">
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>899113</v>
       </c>
-      <c r="C24" s="2">
+      <c r="B24" s="2">
         <v>35950</v>
       </c>
+      <c r="C24">
+        <v>523686</v>
+      </c>
       <c r="D24">
-        <v>523686</v>
+        <v>2</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -1401,75 +1332,72 @@
         <v>2</v>
       </c>
       <c r="G24">
-        <v>2</v>
-      </c>
-      <c r="H24">
         <v>899113</v>
       </c>
-      <c r="I24" s="2">
+      <c r="H24" s="2">
         <v>35950</v>
       </c>
+      <c r="I24">
+        <v>448547</v>
+      </c>
       <c r="J24">
-        <v>448547</v>
+        <v>3</v>
       </c>
       <c r="K24">
         <v>3</v>
       </c>
       <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>899113</v>
+      </c>
+      <c r="N24" s="2">
+        <v>35950</v>
+      </c>
+      <c r="O24">
+        <v>671293</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>2</v>
+      </c>
+      <c r="R24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>922196</v>
+      </c>
+      <c r="B25" s="2">
+        <v>36020</v>
+      </c>
+      <c r="C25">
+        <v>792204</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
         <v>3</v>
       </c>
-      <c r="M24">
-        <v>1</v>
-      </c>
-      <c r="N24">
-        <v>899113</v>
-      </c>
-      <c r="O24" s="2">
-        <v>35950</v>
-      </c>
-      <c r="P24">
-        <v>671293</v>
-      </c>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-      <c r="R24">
-        <v>2</v>
-      </c>
-      <c r="S24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25">
+      <c r="G25">
         <v>922196</v>
       </c>
-      <c r="C25" s="2">
+      <c r="H25" s="2">
         <v>36020</v>
       </c>
-      <c r="D25">
-        <v>792204</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="G25">
+      <c r="I25">
+        <v>383441</v>
+      </c>
+      <c r="J25">
         <v>3</v>
-      </c>
-      <c r="H25">
-        <v>922196</v>
-      </c>
-      <c r="I25" s="2">
-        <v>36020</v>
-      </c>
-      <c r="J25">
-        <v>383441</v>
       </c>
       <c r="K25">
         <v>3</v>
@@ -1478,74 +1406,68 @@
         <v>3</v>
       </c>
       <c r="M25">
-        <v>3</v>
-      </c>
-      <c r="N25">
         <v>922196</v>
       </c>
-      <c r="O25" s="2">
+      <c r="N25" s="2">
         <v>36020</v>
       </c>
+      <c r="O25">
+        <v>363835</v>
+      </c>
       <c r="P25">
-        <v>363835</v>
+        <v>2</v>
       </c>
       <c r="Q25">
-        <v>2</v>
+        <v>-6</v>
       </c>
       <c r="R25">
         <v>-6</v>
       </c>
-      <c r="S25">
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>936316</v>
+      </c>
+      <c r="B26" s="2">
+        <v>37918</v>
+      </c>
+      <c r="C26">
+        <v>198487</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>936316</v>
+      </c>
+      <c r="N26" s="2">
+        <v>37918</v>
+      </c>
+      <c r="O26">
+        <v>443633</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+      <c r="Q26">
         <v>-6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>936316</v>
-      </c>
-      <c r="C26" s="2">
-        <v>37918</v>
-      </c>
-      <c r="D26">
-        <v>198487</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="N26">
-        <v>936316</v>
-      </c>
-      <c r="O26" s="2">
-        <v>37918</v>
-      </c>
-      <c r="P26">
-        <v>443633</v>
-      </c>
-      <c r="Q26">
-        <v>2</v>
       </c>
       <c r="R26">
         <v>-6</v>
       </c>
-      <c r="S26">
-        <v>-6</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:S27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:R27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="3">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="M1:R1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1568,82 +1490,82 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1667,121 +1589,121 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
       <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
       <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
         <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
       <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
         <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
       <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
         <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
       <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1803,42 +1725,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
         <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1866,162 +1788,162 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" t="s">
         <v>68</v>
       </c>
-      <c r="F2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>69</v>
       </c>
-      <c r="H2" t="s">
-        <v>70</v>
-      </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>72</v>
-      </c>
-      <c r="J3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" t="s">
         <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
         <v>76</v>
       </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="J5" t="s">
         <v>68</v>
-      </c>
-      <c r="F5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" t="s">
-        <v>77</v>
-      </c>
-      <c r="J5" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>